<commit_message>
image included and ui changed
</commit_message>
<xml_diff>
--- a/Engine/data/datasheet/ui_parameter.xlsx
+++ b/Engine/data/datasheet/ui_parameter.xlsx
@@ -3,24 +3,30 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29790E2F-6EA9-48FD-A4A9-5E2E3348ABBE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A2644F8-8592-43E9-A026-2DFE1A57C25D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32085" yWindow="1455" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1050" yWindow="1020" windowWidth="12420" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="21">
   <si>
     <t>이미지 원래 사이즈를 사용하고 싶으면 0</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -58,26 +64,10 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>item_bar.png</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ITEM_BAR</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>hpbar_front.png</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>PLAYER_HPBAR_FRONT</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>hpbar_back.png</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>PLAYER_HPBAR_BACK</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -95,6 +85,30 @@
   </si>
   <si>
     <t>BOSS_HPBAR_BACK</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PLAYER_TIMER</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>boss_hp_back.png</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>boss_hp_front.png</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>timer2.png</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>player_hp_back.png</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>player_hp_front.png</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -512,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -527,10 +541,10 @@
         <v>8</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -538,7 +552,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1"/>
     </row>
@@ -547,7 +561,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="4">
-        <v>960</v>
+        <v>1423</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -556,7 +570,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C4" s="1"/>
     </row>
@@ -565,7 +579,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="4">
-        <v>729</v>
+        <v>0</v>
       </c>
       <c r="C5" s="1"/>
     </row>
@@ -574,7 +588,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="2">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="C6" s="1"/>
     </row>
@@ -583,10 +597,10 @@
         <v>8</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -594,7 +608,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C8" s="1"/>
     </row>
@@ -603,7 +617,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="4">
-        <v>960</v>
+        <v>1442</v>
       </c>
       <c r="C9" s="1"/>
     </row>
@@ -612,7 +626,7 @@
         <v>3</v>
       </c>
       <c r="B10" s="4">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C10" s="1"/>
     </row>
@@ -621,7 +635,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="4">
-        <v>729</v>
+        <v>426</v>
       </c>
       <c r="C11" s="1"/>
     </row>
@@ -630,7 +644,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="2">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="C12" s="1"/>
     </row>
@@ -639,7 +653,7 @@
         <v>8</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C13" s="1"/>
     </row>
@@ -648,7 +662,7 @@
         <v>6</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C14" s="1"/>
     </row>
@@ -657,7 +671,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="4">
-        <v>960</v>
+        <v>125</v>
       </c>
       <c r="C15" s="1"/>
     </row>
@@ -666,7 +680,7 @@
         <v>3</v>
       </c>
       <c r="B16" s="4">
-        <v>1030</v>
+        <v>1008</v>
       </c>
       <c r="C16" s="1"/>
     </row>
@@ -675,7 +689,7 @@
         <v>2</v>
       </c>
       <c r="B17" s="4">
-        <v>729</v>
+        <v>0</v>
       </c>
       <c r="C17" s="1"/>
     </row>
@@ -684,7 +698,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="2">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="C18" s="1"/>
     </row>
@@ -693,7 +707,7 @@
         <v>8</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C19" s="1"/>
     </row>
@@ -702,7 +716,7 @@
         <v>6</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C20" s="1"/>
     </row>
@@ -711,7 +725,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="4">
-        <v>960</v>
+        <v>139</v>
       </c>
       <c r="C21" s="1"/>
     </row>
@@ -720,7 +734,7 @@
         <v>3</v>
       </c>
       <c r="B22" s="4">
-        <v>1030</v>
+        <v>1012.5</v>
       </c>
       <c r="C22" s="1"/>
     </row>
@@ -729,7 +743,7 @@
         <v>2</v>
       </c>
       <c r="B23" s="4">
-        <v>729</v>
+        <v>282</v>
       </c>
       <c r="C23" s="1"/>
     </row>
@@ -738,7 +752,7 @@
         <v>1</v>
       </c>
       <c r="B24" s="2">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="C24" s="1"/>
     </row>
@@ -747,7 +761,7 @@
         <v>8</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C25" s="1"/>
     </row>
@@ -756,7 +770,7 @@
         <v>6</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C26" s="1"/>
     </row>
@@ -765,7 +779,7 @@
         <v>4</v>
       </c>
       <c r="B27" s="4">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C27" s="1"/>
     </row>
@@ -774,11 +788,9 @@
         <v>3</v>
       </c>
       <c r="B28" s="4">
-        <v>170</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>0</v>
-      </c>
+        <v>771</v>
+      </c>
+      <c r="C28" s="1"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
@@ -798,63 +810,55 @@
       <c r="B30" s="2">
         <v>0</v>
       </c>
-      <c r="C30" s="1"/>
+      <c r="C30" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C31" s="1"/>
+        <v>15</v>
+      </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C32" s="1"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B33" s="4">
-        <v>10</v>
-      </c>
-      <c r="C33" s="1"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B34" s="4">
-        <v>100</v>
-      </c>
-      <c r="C34" s="1"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B35" s="4">
         <v>0</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="36" spans="1:2" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B36" s="2">
-        <v>0</v>
-      </c>
-      <c r="C36" s="1" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
boss pattern sync fix
</commit_message>
<xml_diff>
--- a/Engine/data/datasheet/ui_parameter.xlsx
+++ b/Engine/data/datasheet/ui_parameter.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3776520B-0270-4560-9008-A4D9419BA92C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B542BE5-C02A-486D-85D0-9FEC7DBABDD9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="3900" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -533,8 +533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -624,7 +624,7 @@
         <v>3</v>
       </c>
       <c r="B9" s="4">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="C9" s="1"/>
     </row>
@@ -633,7 +633,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="4">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C10" s="1"/>
     </row>
@@ -642,7 +642,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="4">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="C11" s="1"/>
     </row>
@@ -838,7 +838,7 @@
         <v>3</v>
       </c>
       <c r="B33" s="4">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -854,7 +854,7 @@
         <v>1</v>
       </c>
       <c r="B35" s="4">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
player resurrection count image inserted
</commit_message>
<xml_diff>
--- a/Engine/data/datasheet/ui_parameter.xlsx
+++ b/Engine/data/datasheet/ui_parameter.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B542BE5-C02A-486D-85D0-9FEC7DBABDD9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B8DA8A-0AF7-4801-8134-31D7F0F47AFE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="26">
   <si>
     <t>Size_Y</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -116,6 +116,18 @@
   </si>
   <si>
     <t>title.png</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>RESURRECTION_COUNT1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>RESURRECTION_COUNT2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>resurrection.png</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -531,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C54"/>
+  <dimension ref="A1:C66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -568,7 +580,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="4">
-        <v>960</v>
+        <v>710</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -624,7 +636,7 @@
         <v>3</v>
       </c>
       <c r="B9" s="4">
-        <v>977</v>
+        <v>725</v>
       </c>
       <c r="C9" s="1"/>
     </row>
@@ -633,7 +645,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="4">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C10" s="1"/>
     </row>
@@ -642,7 +654,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="4">
-        <v>427</v>
+        <v>432</v>
       </c>
       <c r="C11" s="1"/>
     </row>
@@ -651,7 +663,7 @@
         <v>0</v>
       </c>
       <c r="B12" s="2">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C12" s="1"/>
     </row>
@@ -854,7 +866,7 @@
         <v>1</v>
       </c>
       <c r="B35" s="4">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -934,7 +946,7 @@
         <v>3</v>
       </c>
       <c r="B45" s="4">
-        <v>1415</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
@@ -950,7 +962,7 @@
         <v>1</v>
       </c>
       <c r="B47" s="4">
-        <v>282</v>
+        <v>284</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -1007,6 +1019,102 @@
       </c>
       <c r="B54" s="2">
         <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B57" s="4">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B58" s="4">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B59" s="4">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B60" s="2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B63" s="4">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B64" s="4">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B65" s="4">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B66" s="2">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>